<commit_message>
18:19 save. newly added kmeans clustering
</commit_message>
<xml_diff>
--- a/notebooks/notes.xlsx
+++ b/notebooks/notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicacurley/Desktop/galvanize_dsi/capstones/Jeopardy_nlp/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20C234D1-2D24-9242-907C-174DFC344616}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A874D2C-7940-8F4D-8019-438115340D1F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4800" yWindow="460" windowWidth="28040" windowHeight="17440" xr2:uid="{5297B969-6212-EA40-ACF0-2478C497FFD7}"/>
+    <workbookView xWindow="19320" yWindow="3860" windowWidth="14280" windowHeight="15960" xr2:uid="{5297B969-6212-EA40-ACF0-2478C497FFD7}"/>
   </bookViews>
   <sheets>
     <sheet name="keep track" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="38">
   <si>
     <t>am_assignment_nlp.ipynb</t>
   </si>
@@ -68,16 +68,111 @@
   </si>
   <si>
     <t>https://scikit-learn.org/stable/modules/generated/sklearn.feature_extraction.text.CountVectorizer.html</t>
+  </si>
+  <si>
+    <t>Colormaps: https://matplotlib.org/tutorials/colors/colormaps.html</t>
+  </si>
+  <si>
+    <t>Supervised </t>
+  </si>
+  <si>
+    <t>For predicting high value vs. low value per question in regular tournament </t>
+  </si>
+  <si>
+    <t>Make column that combines question and answer</t>
+  </si>
+  <si>
+    <t>That column  = x</t>
+  </si>
+  <si>
+    <t>Make column of high, avg, low value</t>
+  </si>
+  <si>
+    <t>That column = y</t>
+  </si>
+  <si>
+    <t>Train test split on these </t>
+  </si>
+  <si>
+    <t>Fit transform a CountVectorizer on the x_train and y_train</t>
+  </si>
+  <si>
+    <t>Predicting high value vs. low value by tournament </t>
+  </si>
+  <si>
+    <t>Use the same question and answer combined column</t>
+  </si>
+  <si>
+    <t>Make column for reg, easy_special, hard_special depending on notes</t>
+  </si>
+  <si>
+    <t>Train test split on those columns</t>
+  </si>
+  <si>
+    <t>Fit transform a countvectorizer </t>
+  </si>
+  <si>
+    <t>Try different classifiers </t>
+  </si>
+  <si>
+    <t>Test by using </t>
+  </si>
+  <si>
+    <t>Unsupervised - classifying meta-categories using NMF to see the latent topics </t>
+  </si>
+  <si>
+    <t>To Do</t>
+  </si>
+  <si>
+    <t>Tournament class:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attribute </t>
+  </si>
+  <si>
+    <t>data class</t>
+  </si>
+  <si>
+    <t xml:space="preserve">subset of my data is tournamnet </t>
+  </si>
+  <si>
+    <t>data.regular on my train_test_split</t>
+  </si>
+  <si>
+    <t>data.tournament etc</t>
+  </si>
+  <si>
+    <t>jeopardydata = data.df</t>
+  </si>
+  <si>
+    <t xml:space="preserve">naïve bayes to classify the question to the values </t>
+  </si>
+  <si>
+    <t>classifier = cluster with knn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -100,13 +195,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -419,24 +518,161 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD3E849-7AE9-8E45-9316-282A2B564A0B}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <selection activeCell="A46" sqref="A46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="17" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>37</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FDEF45-82B4-584D-99B8-D7ED4DA7397B}">
-  <dimension ref="A3:A20"/>
+  <dimension ref="A3:A28"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,7 +721,7 @@
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
     </row>
@@ -499,7 +735,15 @@
         <v>10</v>
       </c>
     </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A28" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A18" r:id="rId1" xr:uid="{47439E67-4FBE-9F46-A9D7-A69AF49BDA56}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added csv, fixed word count difficulty image
</commit_message>
<xml_diff>
--- a/notebooks/notes.xlsx
+++ b/notebooks/notes.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicacurley/Desktop/galvanize_dsi/capstones/Jeopardy_nlp/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99AF3EBE-A39A-E043-BCFC-2BCEF6E10FE5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2C8112F-6733-6849-8C31-E53EE7568F62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18820" xr2:uid="{5297B969-6212-EA40-ACF0-2478C497FFD7}"/>
+    <workbookView xWindow="60" yWindow="7360" windowWidth="33600" windowHeight="18820" activeTab="1" xr2:uid="{5297B969-6212-EA40-ACF0-2478C497FFD7}"/>
   </bookViews>
   <sheets>
     <sheet name="keep track" sheetId="1" r:id="rId1"/>
-    <sheet name="Resources" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId2"/>
+    <sheet name="Resources" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="93">
   <si>
     <t>am_assignment_nlp.ipynb</t>
   </si>
@@ -495,12 +496,15 @@
   <si>
     <t>write a wordcloud function for my topics and weights and size with a factor x weights</t>
   </si>
+  <si>
+    <t>rename "category' to 'j-category'</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -591,6 +595,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Courier New"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -613,7 +623,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
@@ -670,6 +680,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -987,8 +998,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAD3E849-7AE9-8E45-9316-282A2B564A0B}">
   <dimension ref="A1:X46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+    <sheetView topLeftCell="M3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6:T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1137,7 +1148,9 @@
       <c r="L5" s="5"/>
       <c r="M5" s="5"/>
       <c r="N5" s="7"/>
-      <c r="S5" s="20"/>
+      <c r="S5" s="20" t="s">
+        <v>92</v>
+      </c>
       <c r="T5" s="20"/>
       <c r="U5" s="7"/>
       <c r="V5" s="7"/>
@@ -1944,6 +1957,38 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595D5075-C4DA-F147-8D2C-82ACD2EE2203}">
+  <dimension ref="A5:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A2:A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="81" customWidth="1"/>
+    <col min="2" max="2" width="23.5" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="22"/>
+    </row>
+    <row r="6" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="22"/>
+    </row>
+    <row r="7" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="22"/>
+    </row>
+    <row r="8" spans="1:1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="22"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0FDEF45-82B4-584D-99B8-D7ED4DA7397B}">
   <dimension ref="A3:E28"/>
   <sheetViews>
@@ -2052,7 +2097,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{184E43A1-D413-4F4E-9C63-9B17613F616B}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
docstrings and minor fixes to readme
</commit_message>
<xml_diff>
--- a/notebooks/notes.xlsx
+++ b/notebooks/notes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jessicacurley/Desktop/galvanize_dsi/capstones/Jeopardy_nlp/notebooks/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5653DAE-2FB1-E748-9488-49D98060AC69}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF8ED707-9611-024A-983F-7DD5F224F49B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="100" yWindow="460" windowWidth="33600" windowHeight="18820" activeTab="1" xr2:uid="{5297B969-6212-EA40-ACF0-2478C497FFD7}"/>
+    <workbookView xWindow="20" yWindow="480" windowWidth="33600" windowHeight="18820" activeTab="1" xr2:uid="{5297B969-6212-EA40-ACF0-2478C497FFD7}"/>
   </bookViews>
   <sheets>
     <sheet name="keep track" sheetId="1" r:id="rId1"/>
@@ -1975,7 +1975,7 @@
   <dimension ref="A2:A8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>